<commit_message>
adicao de metodo OCR para leitura da nota impressa.
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelpn\PycharmProjects\automacao_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF17C1FD-268E-46E0-B9CA-25E0409C0F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01267DA6-04EE-4CEB-B523-3C37E62F7998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25905" yWindow="930" windowWidth="11745" windowHeight="12345" xr2:uid="{AAEA7E11-244B-41D9-B354-0EAAB43709D4}"/>
+    <workbookView xWindow="9405" yWindow="570" windowWidth="11745" windowHeight="12345" xr2:uid="{AAEA7E11-244B-41D9-B354-0EAAB43709D4}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Código</t>
   </si>
@@ -180,6 +180,45 @@
   </si>
   <si>
     <t>estrela</t>
+  </si>
+  <si>
+    <t>BELINELLI 2</t>
+  </si>
+  <si>
+    <t>BELINELLI 3</t>
+  </si>
+  <si>
+    <t>BELINELLI 1</t>
+  </si>
+  <si>
+    <t>belinelli 2</t>
+  </si>
+  <si>
+    <t>belinelli 1</t>
+  </si>
+  <si>
+    <t>belinelli 3</t>
+  </si>
+  <si>
+    <t>belinelli 4</t>
+  </si>
+  <si>
+    <t>BELINELLI 4</t>
+  </si>
+  <si>
+    <t>opini</t>
+  </si>
+  <si>
+    <t>OPINI OPINI</t>
+  </si>
+  <si>
+    <t>TITI</t>
+  </si>
+  <si>
+    <t>titi</t>
+  </si>
+  <si>
+    <t>opini opini</t>
   </si>
 </sst>
 </file>
@@ -574,13 +613,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22B1096-DDE8-45EA-9DCD-EE6EF89604B1}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -607,20 +653,18 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
       </c>
       <c r="C2" s="5">
-        <v>18</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="8">
-        <v>14</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="1">
         <v>1</v>
       </c>
@@ -636,13 +680,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -661,13 +705,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -685,15 +729,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5">
-        <v>6</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5">
@@ -710,15 +748,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5">
-        <v>11.2</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="1">
@@ -860,6 +892,12 @@
       <c r="G13" t="s">
         <v>15</v>
       </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -873,6 +911,12 @@
       <c r="G14" t="s">
         <v>16</v>
       </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -886,6 +930,12 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
+      <c r="I15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -899,8 +949,14 @@
       <c r="G16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -912,8 +968,14 @@
       <c r="G17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -925,8 +987,14 @@
       <c r="G18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -939,7 +1007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -952,7 +1020,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4"/>
       <c r="C21" s="6"/>
@@ -965,7 +1033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4"/>
       <c r="C22" s="6"/>
@@ -978,7 +1046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="6"/>
@@ -991,7 +1059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="6"/>

</xml_diff>